<commit_message>
Transparent logo, unnecessary alerts removed, 2nd file chooser with 1st FC path
</commit_message>
<xml_diff>
--- a/data/Tickets_nao_tratados.xlsx-FINAL REPORT.xlsx
+++ b/data/Tickets_nao_tratados.xlsx-FINAL REPORT.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Number</t>
   </si>
@@ -32,22 +32,19 @@
     <t>Updated on</t>
   </si>
   <si>
-    <t>TASK4</t>
+    <t>TASK1509262</t>
   </si>
   <si>
-    <t>Victor Barcelos-External</t>
+    <t>Rafael Goncalves Reis</t>
   </si>
   <si>
-    <t>DSS - Brazil - Macaé</t>
+    <t>DSS - Brazil - Rio de Janeiro / Cidade Nova</t>
   </si>
   <si>
     <t>Awaiting</t>
   </si>
   <si>
     <t>06-10-2021</t>
-  </si>
-  <si>
-    <t>08-10-2021</t>
   </si>
 </sst>
 </file>
@@ -135,7 +132,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>